<commit_message>
April 10th post and update table renderings
</commit_message>
<xml_diff>
--- a/master_files/2023_draft_big_boards.xlsx
+++ b/master_files/2023_draft_big_boards.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Bushman\Documents\R\jabber-jazz-content-notes\master_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Repos\jabber-jazz-content-notes\master_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FAD0FA-D5C8-4390-9B9E-43376D18BB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36F6678-3FB2-40BA-AF9B-56739D9803E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{3F3E3C4B-A1D3-4C9C-9B2F-6D892D359046}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3F3E3C4B-A1D3-4C9C-9B2F-6D892D359046}"/>
   </bookViews>
   <sheets>
     <sheet name="Josh-Roberts" sheetId="1" r:id="rId1"/>
     <sheet name="Leif-Thulin" sheetId="2" r:id="rId2"/>
     <sheet name="Mark" sheetId="3" r:id="rId3"/>
+    <sheet name="AJ" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="133">
   <si>
     <t>pick</t>
   </si>
@@ -430,22 +431,13 @@
     <t>Gonzaga</t>
   </si>
   <si>
-    <t>Tier 1</t>
-  </si>
-  <si>
-    <t>Tier 2</t>
-  </si>
-  <si>
-    <t>Tier 3</t>
-  </si>
-  <si>
-    <t>Tier 4</t>
-  </si>
-  <si>
-    <t>Tier 5</t>
-  </si>
-  <si>
-    <t>Tier 6</t>
+    <t>Bilal Coulibaly</t>
+  </si>
+  <si>
+    <t>Kobe Bufkin</t>
+  </si>
+  <si>
+    <t>230 lbs</t>
   </si>
 </sst>
 </file>
@@ -2650,8 +2642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430CCBA0-2015-4C49-8928-DF5D7A4897ED}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2700,8 +2692,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>130</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -2729,8 +2721,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>131</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -2758,8 +2750,8 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>132</v>
+      <c r="B4">
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -2787,8 +2779,8 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>132</v>
+      <c r="B5">
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>36</v>
@@ -2816,8 +2808,8 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>132</v>
+      <c r="B6">
+        <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
@@ -2845,8 +2837,8 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>133</v>
+      <c r="B7">
+        <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>44</v>
@@ -2874,8 +2866,8 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>133</v>
+      <c r="B8">
+        <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
@@ -2903,8 +2895,8 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>133</v>
+      <c r="B9">
+        <v>4</v>
       </c>
       <c r="C9" t="s">
         <v>48</v>
@@ -2932,8 +2924,8 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>133</v>
+      <c r="B10">
+        <v>4</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
@@ -2961,8 +2953,8 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>133</v>
+      <c r="B11">
+        <v>4</v>
       </c>
       <c r="C11" t="s">
         <v>54</v>
@@ -2990,8 +2982,8 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>134</v>
+      <c r="B12">
+        <v>5</v>
       </c>
       <c r="C12" t="s">
         <v>60</v>
@@ -3019,8 +3011,8 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>134</v>
+      <c r="B13">
+        <v>5</v>
       </c>
       <c r="C13" t="s">
         <v>109</v>
@@ -3048,8 +3040,8 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>134</v>
+      <c r="B14">
+        <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>111</v>
@@ -3077,8 +3069,8 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>134</v>
+      <c r="B15">
+        <v>5</v>
       </c>
       <c r="C15" t="s">
         <v>64</v>
@@ -3106,8 +3098,8 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>134</v>
+      <c r="B16">
+        <v>5</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
@@ -3135,8 +3127,8 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>134</v>
+      <c r="B17">
+        <v>5</v>
       </c>
       <c r="C17" t="s">
         <v>51</v>
@@ -3164,8 +3156,8 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>135</v>
+      <c r="B18">
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>104</v>
@@ -3193,8 +3185,8 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>135</v>
+      <c r="B19">
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>67</v>
@@ -3222,8 +3214,8 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>135</v>
+      <c r="B20">
+        <v>6</v>
       </c>
       <c r="C20" t="s">
         <v>110</v>
@@ -3251,8 +3243,8 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>135</v>
+      <c r="B21">
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>56</v>
@@ -3280,8 +3272,8 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>135</v>
+      <c r="B22">
+        <v>6</v>
       </c>
       <c r="C22" t="s">
         <v>90</v>
@@ -3309,8 +3301,8 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>135</v>
+      <c r="B23">
+        <v>6</v>
       </c>
       <c r="C23" t="s">
         <v>80</v>
@@ -3338,8 +3330,8 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>135</v>
+      <c r="B24">
+        <v>6</v>
       </c>
       <c r="C24" t="s">
         <v>124</v>
@@ -3367,8 +3359,8 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>135</v>
+      <c r="B25">
+        <v>6</v>
       </c>
       <c r="C25" t="s">
         <v>62</v>
@@ -3396,8 +3388,8 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>135</v>
+      <c r="B26">
+        <v>6</v>
       </c>
       <c r="C26" t="s">
         <v>108</v>
@@ -3425,8 +3417,8 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>135</v>
+      <c r="B27">
+        <v>6</v>
       </c>
       <c r="C27" t="s">
         <v>125</v>
@@ -3454,8 +3446,8 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>135</v>
+      <c r="B28">
+        <v>6</v>
       </c>
       <c r="C28" t="s">
         <v>107</v>
@@ -3483,8 +3475,8 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>135</v>
+      <c r="B29">
+        <v>6</v>
       </c>
       <c r="C29" t="s">
         <v>71</v>
@@ -3512,8 +3504,8 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>135</v>
+      <c r="B30">
+        <v>6</v>
       </c>
       <c r="C30" t="s">
         <v>126</v>
@@ -3535,6 +3527,866 @@
       </c>
       <c r="I30" s="1">
         <v>37364</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E65D78-84F0-48B7-951C-45EDF82BBBBB}">
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1">
+        <v>37990</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="1">
+        <v>38020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="1">
+        <v>38176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="1">
+        <v>37651</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="1">
+        <v>37582</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="1">
+        <v>37651</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="1">
+        <v>37868</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="1">
+        <v>37932</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="1">
+        <v>38006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="1">
+        <v>38338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="1">
+        <v>38200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" t="s">
+        <v>121</v>
+      </c>
+      <c r="I13" s="1">
+        <v>37947</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="1">
+        <v>38095</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="1">
+        <v>37878</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="1">
+        <v>37945</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="1">
+        <v>37375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="1">
+        <v>37933</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="1">
+        <v>37791</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" t="s">
+        <v>119</v>
+      </c>
+      <c r="I20" s="1">
+        <v>37924</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="1">
+        <v>36757</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" t="s">
+        <v>132</v>
+      </c>
+      <c r="I22" s="1">
+        <v>38194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="1">
+        <v>38138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24" s="1">
+        <v>37404</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="1">
+        <v>37464</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="1">
+        <v>37885</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" t="s">
+        <v>117</v>
+      </c>
+      <c r="I27" s="1">
+        <v>38182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" s="1">
+        <v>38079</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" t="s">
+        <v>100</v>
+      </c>
+      <c r="H29" t="s">
+        <v>132</v>
+      </c>
+      <c r="I29" s="1">
+        <v>38029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Episode from May 26
</commit_message>
<xml_diff>
--- a/master_files/2023_draft_big_boards.xlsx
+++ b/master_files/2023_draft_big_boards.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Repos\jabber-jazz-content-notes\master_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36F6678-3FB2-40BA-AF9B-56739D9803E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979720E1-15EC-4EBD-BC4D-E45103D7310D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3F3E3C4B-A1D3-4C9C-9B2F-6D892D359046}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{3F3E3C4B-A1D3-4C9C-9B2F-6D892D359046}"/>
   </bookViews>
   <sheets>
     <sheet name="Josh-Roberts" sheetId="1" r:id="rId1"/>
     <sheet name="Leif-Thulin" sheetId="2" r:id="rId2"/>
     <sheet name="Mark" sheetId="3" r:id="rId3"/>
     <sheet name="AJ" sheetId="4" r:id="rId4"/>
+    <sheet name="Adam-Bushman" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="148">
   <si>
     <t>pick</t>
   </si>
@@ -438,6 +439,51 @@
   </si>
   <si>
     <t>230 lbs</t>
+  </si>
+  <si>
+    <t>James Nnaji</t>
+  </si>
+  <si>
+    <t>Andre Jackson</t>
+  </si>
+  <si>
+    <t>Ricky Council IV</t>
+  </si>
+  <si>
+    <t>Brandin Podziemski</t>
+  </si>
+  <si>
+    <t>Trayce Jackson-Davis</t>
+  </si>
+  <si>
+    <t>Jaime Jaquez Jr.</t>
+  </si>
+  <si>
+    <t>Terrence Shannon Jr.</t>
+  </si>
+  <si>
+    <t>Adem Bona</t>
+  </si>
+  <si>
+    <t>Metropolitans92</t>
+  </si>
+  <si>
+    <t>Barcelona (ACB)</t>
+  </si>
+  <si>
+    <t>Santa Clara</t>
+  </si>
+  <si>
+    <t>245 lbs</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Off: Forward</t>
+  </si>
+  <si>
+    <t>Def: Forward</t>
   </si>
 </sst>
 </file>
@@ -2642,8 +2688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430CCBA0-2015-4C49-8928-DF5D7A4897ED}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4392,4 +4438,1185 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C80E46-0F5C-4BF5-9546-9B686A8E86D5}">
+  <dimension ref="A1:I40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1">
+        <v>37990</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="1">
+        <v>37582</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="1">
+        <v>38020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="1">
+        <v>37868</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="1">
+        <v>38176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="1">
+        <v>37651</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="1">
+        <v>37651</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="1">
+        <v>38006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="1">
+        <v>38338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="1">
+        <v>37932</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>121</v>
+      </c>
+      <c r="I12" s="1">
+        <v>37947</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="1">
+        <v>38200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" s="1">
+        <v>37791</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="1">
+        <v>37464</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="1">
+        <v>37945</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="1">
+        <v>37375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="1">
+        <v>37885</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" t="s">
+        <v>147</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="1">
+        <v>38079</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" t="s">
+        <v>119</v>
+      </c>
+      <c r="I20" s="1">
+        <v>37924</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="1">
+        <v>37933</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="1">
+        <v>37878</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" s="1">
+        <v>38095</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24" s="1">
+        <v>37404</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" t="s">
+        <v>141</v>
+      </c>
+      <c r="G25" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" t="s">
+        <v>132</v>
+      </c>
+      <c r="I25" s="1">
+        <v>38194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>146</v>
+      </c>
+      <c r="E26" t="s">
+        <v>147</v>
+      </c>
+      <c r="F26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="1">
+        <v>36757</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" t="s">
+        <v>146</v>
+      </c>
+      <c r="E27" t="s">
+        <v>147</v>
+      </c>
+      <c r="F27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" t="s">
+        <v>117</v>
+      </c>
+      <c r="I27" s="1">
+        <v>38182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" t="s">
+        <v>122</v>
+      </c>
+      <c r="G28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I28" s="1">
+        <v>38138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" t="s">
+        <v>92</v>
+      </c>
+      <c r="I29" s="1">
+        <v>37621</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" t="s">
+        <v>100</v>
+      </c>
+      <c r="H30" t="s">
+        <v>132</v>
+      </c>
+      <c r="I30" s="1">
+        <v>38029</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>133</v>
+      </c>
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="1">
+        <v>38213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" t="s">
+        <v>147</v>
+      </c>
+      <c r="F32" t="s">
+        <v>127</v>
+      </c>
+      <c r="G32" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" t="s">
+        <v>121</v>
+      </c>
+      <c r="I32" s="1">
+        <v>37208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" t="s">
+        <v>72</v>
+      </c>
+      <c r="H33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I33" s="1">
+        <v>37951</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="1">
+        <v>37106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" t="s">
+        <v>143</v>
+      </c>
+      <c r="G35" t="s">
+        <v>34</v>
+      </c>
+      <c r="H35" t="s">
+        <v>117</v>
+      </c>
+      <c r="I35" s="1">
+        <v>37677</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36" t="s">
+        <v>38</v>
+      </c>
+      <c r="H36" t="s">
+        <v>144</v>
+      </c>
+      <c r="I36" s="1">
+        <v>36578</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" t="s">
+        <v>147</v>
+      </c>
+      <c r="F37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G37" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" t="s">
+        <v>29</v>
+      </c>
+      <c r="I37" s="1">
+        <v>36940</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>139</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" t="s">
+        <v>145</v>
+      </c>
+      <c r="G38" t="s">
+        <v>68</v>
+      </c>
+      <c r="H38" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" s="1">
+        <v>36737</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>116</v>
+      </c>
+      <c r="G39" t="s">
+        <v>72</v>
+      </c>
+      <c r="H39" t="s">
+        <v>29</v>
+      </c>
+      <c r="I39" s="1">
+        <v>37483</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>140</v>
+      </c>
+      <c r="D40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>94</v>
+      </c>
+      <c r="G40" t="s">
+        <v>72</v>
+      </c>
+      <c r="H40" t="s">
+        <v>119</v>
+      </c>
+      <c r="I40" s="1">
+        <v>37708</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Adam's big board
</commit_message>
<xml_diff>
--- a/master_files/2023_draft_big_boards.xlsx
+++ b/master_files/2023_draft_big_boards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Repos\jabber-jazz-content-notes\master_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Bushman\Documents\R\jabber-jazz-content-notes\master_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979720E1-15EC-4EBD-BC4D-E45103D7310D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3B3F2B-ED00-4835-937E-611D8BB5C913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{3F3E3C4B-A1D3-4C9C-9B2F-6D892D359046}"/>
+    <workbookView xWindow="11470" yWindow="0" windowWidth="7820" windowHeight="10170" firstSheet="4" activeTab="4" xr2:uid="{3F3E3C4B-A1D3-4C9C-9B2F-6D892D359046}"/>
   </bookViews>
   <sheets>
     <sheet name="Josh-Roberts" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="193">
   <si>
     <t>pick</t>
   </si>
@@ -474,16 +474,151 @@
     <t>Santa Clara</t>
   </si>
   <si>
-    <t>245 lbs</t>
-  </si>
-  <si>
     <t>Illinois</t>
   </si>
   <si>
-    <t>Off: Forward</t>
-  </si>
-  <si>
-    <t>Def: Forward</t>
+    <t>Nikola Djurisic</t>
+  </si>
+  <si>
+    <t>Jalen Wilson</t>
+  </si>
+  <si>
+    <t>Trey Alexander</t>
+  </si>
+  <si>
+    <t>Keyontae Johnson</t>
+  </si>
+  <si>
+    <t>Judah Mintz</t>
+  </si>
+  <si>
+    <t>Julian Phillips</t>
+  </si>
+  <si>
+    <t>Zach Edey</t>
+  </si>
+  <si>
+    <t>249 lbs</t>
+  </si>
+  <si>
+    <t>218 lbs</t>
+  </si>
+  <si>
+    <t>214 lbs</t>
+  </si>
+  <si>
+    <t>217 lbs</t>
+  </si>
+  <si>
+    <t>187 lbs</t>
+  </si>
+  <si>
+    <t>186 lbs</t>
+  </si>
+  <si>
+    <t>204 lbs</t>
+  </si>
+  <si>
+    <t>224 lbs</t>
+  </si>
+  <si>
+    <t>199 lbs</t>
+  </si>
+  <si>
+    <t>198 lbs</t>
+  </si>
+  <si>
+    <t>196 lbs</t>
+  </si>
+  <si>
+    <t>163 lbs</t>
+  </si>
+  <si>
+    <t>193 lbs</t>
+  </si>
+  <si>
+    <t>208 lbs</t>
+  </si>
+  <si>
+    <t>240 lbs</t>
+  </si>
+  <si>
+    <t>226 lbs</t>
+  </si>
+  <si>
+    <t>221 lbs</t>
+  </si>
+  <si>
+    <t>243 lbs</t>
+  </si>
+  <si>
+    <t>239 lbs</t>
+  </si>
+  <si>
+    <t>176 lbs</t>
+  </si>
+  <si>
+    <t>209 lbs</t>
+  </si>
+  <si>
+    <t>197 lbs</t>
+  </si>
+  <si>
+    <t>306 lbs</t>
+  </si>
+  <si>
+    <t>7'5"</t>
+  </si>
+  <si>
+    <t>6'3"</t>
+  </si>
+  <si>
+    <t>7'3"</t>
+  </si>
+  <si>
+    <t>Iowa State</t>
+  </si>
+  <si>
+    <t>Mega Basket</t>
+  </si>
+  <si>
+    <t>Creighton</t>
+  </si>
+  <si>
+    <t>Kansas State</t>
+  </si>
+  <si>
+    <t>Syracuse</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Purdue</t>
+  </si>
+  <si>
+    <t>Off:Wing</t>
+  </si>
+  <si>
+    <t>Def:Big</t>
+  </si>
+  <si>
+    <t>Def:Wing</t>
+  </si>
+  <si>
+    <t>Off:Guard</t>
+  </si>
+  <si>
+    <t>Def:Guard</t>
+  </si>
+  <si>
+    <t>Off:Forward</t>
+  </si>
+  <si>
+    <t>Def:Forward</t>
+  </si>
+  <si>
+    <t>Off:Big</t>
   </si>
 </sst>
 </file>
@@ -842,20 +977,20 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -884,7 +1019,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -913,7 +1048,7 @@
         <v>37990</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -942,7 +1077,7 @@
         <v>38020</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -971,7 +1106,7 @@
         <v>37651</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1000,7 +1135,7 @@
         <v>38176</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1029,7 +1164,7 @@
         <v>37651</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1058,7 +1193,7 @@
         <v>38095</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1087,7 +1222,7 @@
         <v>37582</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1116,7 +1251,7 @@
         <v>38006</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1145,7 +1280,7 @@
         <v>37868</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1174,7 +1309,7 @@
         <v>38338</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1203,7 +1338,7 @@
         <v>37932</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1232,7 +1367,7 @@
         <v>37878</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1261,7 +1396,7 @@
         <v>37932</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1290,7 +1425,7 @@
         <v>37945</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1319,7 +1454,7 @@
         <v>36757</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1348,7 +1483,7 @@
         <v>37933</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1377,7 +1512,7 @@
         <v>38200</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1406,7 +1541,7 @@
         <v>38049</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1435,7 +1570,7 @@
         <v>37951</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1464,7 +1599,7 @@
         <v>36790</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1493,7 +1628,7 @@
         <v>38097</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1522,7 +1657,7 @@
         <v>37938</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1551,7 +1686,7 @@
         <v>37791</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1580,7 +1715,7 @@
         <v>37897</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1609,7 +1744,7 @@
         <v>37844</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1638,7 +1773,7 @@
         <v>37404</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1667,7 +1802,7 @@
         <v>37621</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1696,7 +1831,7 @@
         <v>38034</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1725,7 +1860,7 @@
         <v>37333</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1767,20 +1902,20 @@
       <selection activeCell="C27" sqref="C27:I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1809,7 +1944,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1838,7 +1973,7 @@
         <v>37990</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1867,7 +2002,7 @@
         <v>38020</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1896,7 +2031,7 @@
         <v>37651</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1925,7 +2060,7 @@
         <v>37651</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1954,7 +2089,7 @@
         <v>37582</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1983,7 +2118,7 @@
         <v>38176</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2012,7 +2147,7 @@
         <v>38338</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2041,7 +2176,7 @@
         <v>37933</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2070,7 +2205,7 @@
         <v>38006</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2099,7 +2234,7 @@
         <v>37932</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2128,7 +2263,7 @@
         <v>38095</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2157,7 +2292,7 @@
         <v>37868</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2186,7 +2321,7 @@
         <v>37878</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2215,7 +2350,7 @@
         <v>37464</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2244,7 +2379,7 @@
         <v>38200</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2273,7 +2408,7 @@
         <v>38024</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2302,7 +2437,7 @@
         <v>37945</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2331,7 +2466,7 @@
         <v>37621</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2360,7 +2495,7 @@
         <v>37483</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2389,7 +2524,7 @@
         <v>38182</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2418,7 +2553,7 @@
         <v>37924</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2447,7 +2582,7 @@
         <v>38097</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2476,7 +2611,7 @@
         <v>36757</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2505,7 +2640,7 @@
         <v>37932</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2534,7 +2669,7 @@
         <v>37947</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2563,7 +2698,7 @@
         <v>38138</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2592,7 +2727,7 @@
         <v>38029</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2621,7 +2756,7 @@
         <v>37951</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2650,7 +2785,7 @@
         <v>38079</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2692,20 +2827,20 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2734,7 +2869,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2763,7 +2898,7 @@
         <v>37990</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2792,7 +2927,7 @@
         <v>38020</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2821,7 +2956,7 @@
         <v>37651</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2850,7 +2985,7 @@
         <v>37582</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2879,7 +3014,7 @@
         <v>37651</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2908,7 +3043,7 @@
         <v>37868</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2937,7 +3072,7 @@
         <v>38176</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2966,7 +3101,7 @@
         <v>38338</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2995,7 +3130,7 @@
         <v>38006</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3024,7 +3159,7 @@
         <v>37878</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3053,7 +3188,7 @@
         <v>37945</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3082,7 +3217,7 @@
         <v>37947</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3111,7 +3246,7 @@
         <v>38079</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3140,7 +3275,7 @@
         <v>37933</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3169,7 +3304,7 @@
         <v>38095</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3198,7 +3333,7 @@
         <v>37932</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3227,7 +3362,7 @@
         <v>37464</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3256,7 +3391,7 @@
         <v>38200</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3285,7 +3420,7 @@
         <v>38138</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3314,7 +3449,7 @@
         <v>37932</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3343,7 +3478,7 @@
         <v>37621</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3372,7 +3507,7 @@
         <v>37791</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3401,7 +3536,7 @@
         <v>37375</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3430,7 +3565,7 @@
         <v>36757</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3459,7 +3594,7 @@
         <v>37924</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3488,7 +3623,7 @@
         <v>38014</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3517,7 +3652,7 @@
         <v>38182</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3546,7 +3681,7 @@
         <v>37951</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3588,13 +3723,13 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3623,7 +3758,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3652,7 +3787,7 @@
         <v>37990</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3681,7 +3816,7 @@
         <v>38020</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3710,7 +3845,7 @@
         <v>38176</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3739,7 +3874,7 @@
         <v>37651</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3768,7 +3903,7 @@
         <v>37582</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3797,7 +3932,7 @@
         <v>37651</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3826,7 +3961,7 @@
         <v>37868</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3855,7 +3990,7 @@
         <v>37932</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3884,7 +4019,7 @@
         <v>38006</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3913,7 +4048,7 @@
         <v>38338</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3942,7 +4077,7 @@
         <v>38200</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3971,7 +4106,7 @@
         <v>37947</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4000,7 +4135,7 @@
         <v>38095</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4029,7 +4164,7 @@
         <v>37878</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4058,7 +4193,7 @@
         <v>37945</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4087,7 +4222,7 @@
         <v>37375</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4116,7 +4251,7 @@
         <v>37933</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4145,7 +4280,7 @@
         <v>37791</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4174,7 +4309,7 @@
         <v>37924</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4203,7 +4338,7 @@
         <v>36757</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4232,7 +4367,7 @@
         <v>38194</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4261,7 +4396,7 @@
         <v>38138</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4290,7 +4425,7 @@
         <v>37404</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4319,7 +4454,7 @@
         <v>37464</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4348,7 +4483,7 @@
         <v>37885</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4377,7 +4512,7 @@
         <v>38182</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4406,7 +4541,7 @@
         <v>38079</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4442,21 +4577,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C80E46-0F5C-4BF5-9546-9B686A8E86D5}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4485,7 +4618,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4496,16 +4629,16 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>185</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>186</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>141</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>175</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
@@ -4514,7 +4647,7 @@
         <v>37990</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4525,10 +4658,10 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>185</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>187</v>
       </c>
       <c r="F3" t="s">
         <v>37</v>
@@ -4543,7 +4676,7 @@
         <v>37582</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4554,10 +4687,10 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>188</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>189</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -4572,7 +4705,7 @@
         <v>38020</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4583,25 +4716,25 @@
         <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>190</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
       <c r="F5" t="s">
         <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="I5" s="1">
         <v>37868</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4612,25 +4745,25 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>185</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>191</v>
       </c>
       <c r="F6" t="s">
         <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="I6" s="1">
         <v>38176</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4641,25 +4774,25 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>185</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>187</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>153</v>
       </c>
       <c r="I7" s="1">
         <v>37651</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4670,25 +4803,25 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>188</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>187</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>154</v>
       </c>
       <c r="I8" s="1">
         <v>37651</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4699,25 +4832,25 @@
         <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>188</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>189</v>
       </c>
       <c r="F9" t="s">
         <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="I9" s="1">
         <v>38006</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4725,28 +4858,28 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>188</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>189</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>176</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="I10" s="1">
-        <v>38338</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37932</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4754,28 +4887,28 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>191</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>154</v>
       </c>
       <c r="I11" s="1">
-        <v>37932</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37947</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4783,28 +4916,28 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>146</v>
+        <v>185</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
       <c r="F12" t="s">
-        <v>120</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="H12" t="s">
-        <v>121</v>
+        <v>154</v>
       </c>
       <c r="I12" s="1">
-        <v>37947</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4812,28 +4945,28 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>188</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>189</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="H13" t="s">
-        <v>69</v>
+        <v>155</v>
       </c>
       <c r="I13" s="1">
-        <v>38200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37791</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4841,28 +4974,28 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>188</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>189</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="H14" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="I14" s="1">
-        <v>37791</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37885</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4870,28 +5003,28 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>185</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>187</v>
       </c>
       <c r="F15" t="s">
-        <v>112</v>
+        <v>58</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="H15" t="s">
-        <v>35</v>
+        <v>155</v>
       </c>
       <c r="I15" s="1">
-        <v>37464</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4899,28 +5032,28 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>185</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>187</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I16" s="1">
-        <v>37945</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37464</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4928,28 +5061,28 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>188</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>189</v>
       </c>
       <c r="F17" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="G17" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="H17" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="I17" s="1">
-        <v>37375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37933</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4957,28 +5090,28 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>188</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>189</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="G18" t="s">
         <v>53</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
+        <v>157</v>
       </c>
       <c r="I18" s="1">
-        <v>37885</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37375</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4986,28 +5119,28 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>188</v>
       </c>
       <c r="E19" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H19" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I19" s="1">
-        <v>38079</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37878</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5015,28 +5148,28 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>188</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>187</v>
       </c>
       <c r="F20" t="s">
-        <v>118</v>
+        <v>61</v>
       </c>
       <c r="G20" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="H20" t="s">
-        <v>119</v>
+        <v>158</v>
       </c>
       <c r="I20" s="1">
-        <v>37924</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37945</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5044,28 +5177,28 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>192</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>186</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G21" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="H21" t="s">
-        <v>35</v>
+        <v>132</v>
       </c>
       <c r="I21" s="1">
-        <v>37933</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38029</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5073,28 +5206,28 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>191</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="G22" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="H22" t="s">
-        <v>47</v>
+        <v>159</v>
       </c>
       <c r="I22" s="1">
-        <v>37878</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38079</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5102,86 +5235,86 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>185</v>
       </c>
       <c r="E23" t="s">
-        <v>18</v>
+        <v>187</v>
       </c>
       <c r="F23" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="G23" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="H23" t="s">
-        <v>35</v>
+        <v>132</v>
       </c>
       <c r="I23" s="1">
-        <v>38095</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>185</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>187</v>
       </c>
       <c r="F24" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="G24" t="s">
         <v>68</v>
       </c>
       <c r="H24" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I24" s="1">
-        <v>37404</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37924</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>130</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>188</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>189</v>
       </c>
       <c r="F25" t="s">
-        <v>141</v>
+        <v>33</v>
       </c>
       <c r="G25" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="H25" t="s">
-        <v>132</v>
+        <v>35</v>
       </c>
       <c r="I25" s="1">
-        <v>38194</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38095</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5189,28 +5322,28 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>146</v>
+        <v>190</v>
       </c>
       <c r="E26" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
       <c r="F26" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="G26" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H26" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="I26" s="1">
-        <v>36757</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37951</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5218,28 +5351,28 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
-        <v>146</v>
+        <v>188</v>
       </c>
       <c r="E27" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="F27" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="G27" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="H27" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="I27" s="1">
-        <v>38182</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37404</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5247,28 +5380,28 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>190</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>191</v>
       </c>
       <c r="F28" t="s">
-        <v>122</v>
+        <v>178</v>
       </c>
       <c r="G28" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H28" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="I28" s="1">
-        <v>38138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36757</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5276,28 +5409,28 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="E29" t="s">
-        <v>18</v>
+        <v>191</v>
       </c>
       <c r="F29" t="s">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="G29" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="H29" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="I29" s="1">
-        <v>37621</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5305,28 +5438,28 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>190</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="F30" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="G30" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="H30" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="I30" s="1">
-        <v>38029</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5337,10 +5470,10 @@
         <v>133</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>192</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>186</v>
       </c>
       <c r="F31" t="s">
         <v>142</v>
@@ -5355,7 +5488,7 @@
         <v>38213</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5363,28 +5496,28 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
       <c r="D32" t="s">
-        <v>146</v>
+        <v>188</v>
       </c>
       <c r="E32" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="F32" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
       <c r="G32" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="H32" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
       <c r="I32" s="1">
-        <v>37208</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36790</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5392,28 +5525,28 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="D33" t="s">
-        <v>146</v>
+        <v>188</v>
       </c>
       <c r="E33" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="F33" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="G33" t="s">
-        <v>72</v>
+        <v>176</v>
       </c>
       <c r="H33" t="s">
-        <v>73</v>
+        <v>163</v>
       </c>
       <c r="I33" s="1">
-        <v>37951</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37621</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5421,199 +5554,518 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>185</v>
       </c>
       <c r="E34" t="s">
-        <v>23</v>
+        <v>187</v>
       </c>
       <c r="F34" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="G34" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="H34" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="I34" s="1">
-        <v>37106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37677</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
+        <v>185</v>
       </c>
       <c r="E35" t="s">
-        <v>23</v>
+        <v>187</v>
       </c>
       <c r="F35" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="G35" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="H35" t="s">
-        <v>117</v>
+        <v>164</v>
       </c>
       <c r="I35" s="1">
-        <v>37677</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>185</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>187</v>
       </c>
       <c r="F36" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="G36" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="H36" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="I36" s="1">
-        <v>36578</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38040</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D37" t="s">
-        <v>146</v>
+        <v>185</v>
       </c>
       <c r="E37" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="F37" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G37" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H37" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="I37" s="1">
-        <v>36940</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>192</v>
       </c>
       <c r="E38" t="s">
-        <v>23</v>
+        <v>186</v>
       </c>
       <c r="F38" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="G38" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="H38" t="s">
-        <v>50</v>
+        <v>166</v>
       </c>
       <c r="I38" s="1">
-        <v>36737</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36578</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
       <c r="D39" t="s">
-        <v>57</v>
+        <v>185</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="F39" t="s">
-        <v>116</v>
+        <v>61</v>
       </c>
       <c r="G39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H39" t="s">
-        <v>29</v>
+        <v>132</v>
       </c>
       <c r="I39" s="1">
-        <v>37483</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36834</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D40" t="s">
-        <v>57</v>
+        <v>190</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="F40" t="s">
         <v>94</v>
       </c>
       <c r="G40" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H40" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="I40" s="1">
+        <v>36940</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>139</v>
+      </c>
+      <c r="D41" t="s">
+        <v>185</v>
+      </c>
+      <c r="E41" t="s">
+        <v>187</v>
+      </c>
+      <c r="F41" t="s">
+        <v>144</v>
+      </c>
+      <c r="G41" t="s">
+        <v>68</v>
+      </c>
+      <c r="H41" t="s">
+        <v>47</v>
+      </c>
+      <c r="I41" s="1">
+        <v>36737</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" t="s">
+        <v>192</v>
+      </c>
+      <c r="E42" t="s">
+        <v>186</v>
+      </c>
+      <c r="F42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G42" t="s">
+        <v>38</v>
+      </c>
+      <c r="H42" t="s">
+        <v>168</v>
+      </c>
+      <c r="I42" s="1">
+        <v>37483</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" t="s">
+        <v>192</v>
+      </c>
+      <c r="E43" t="s">
+        <v>186</v>
+      </c>
+      <c r="F43" t="s">
+        <v>94</v>
+      </c>
+      <c r="G43" t="s">
+        <v>46</v>
+      </c>
+      <c r="H43" t="s">
+        <v>169</v>
+      </c>
+      <c r="I43" s="1">
         <v>37708</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" t="s">
+        <v>188</v>
+      </c>
+      <c r="E44" t="s">
+        <v>189</v>
+      </c>
+      <c r="F44" t="s">
+        <v>180</v>
+      </c>
+      <c r="G44" t="s">
+        <v>176</v>
+      </c>
+      <c r="H44" t="s">
+        <v>35</v>
+      </c>
+      <c r="I44" s="1">
+        <v>37743</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>148</v>
+      </c>
+      <c r="D45" t="s">
+        <v>190</v>
+      </c>
+      <c r="E45" t="s">
+        <v>191</v>
+      </c>
+      <c r="F45" t="s">
+        <v>181</v>
+      </c>
+      <c r="G45" t="s">
+        <v>53</v>
+      </c>
+      <c r="H45" t="s">
+        <v>170</v>
+      </c>
+      <c r="I45" s="1">
+        <v>36670</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" t="s">
+        <v>192</v>
+      </c>
+      <c r="E46" t="s">
+        <v>186</v>
+      </c>
+      <c r="F46" t="s">
+        <v>84</v>
+      </c>
+      <c r="G46" t="s">
+        <v>46</v>
+      </c>
+      <c r="H46" t="s">
+        <v>164</v>
+      </c>
+      <c r="I46" s="1">
+        <v>37897</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>149</v>
+      </c>
+      <c r="D47" t="s">
+        <v>188</v>
+      </c>
+      <c r="E47" t="s">
+        <v>189</v>
+      </c>
+      <c r="F47" t="s">
+        <v>182</v>
+      </c>
+      <c r="G47" t="s">
+        <v>176</v>
+      </c>
+      <c r="H47" t="s">
+        <v>171</v>
+      </c>
+      <c r="I47" s="1">
+        <v>37812</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" t="s">
+        <v>190</v>
+      </c>
+      <c r="E48" t="s">
+        <v>187</v>
+      </c>
+      <c r="F48" t="s">
+        <v>33</v>
+      </c>
+      <c r="G48" t="s">
+        <v>68</v>
+      </c>
+      <c r="H48" t="s">
+        <v>158</v>
+      </c>
+      <c r="I48" s="1">
+        <v>38049</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>126</v>
+      </c>
+      <c r="D49" t="s">
+        <v>188</v>
+      </c>
+      <c r="E49" t="s">
+        <v>189</v>
+      </c>
+      <c r="F49" t="s">
+        <v>129</v>
+      </c>
+      <c r="G49" t="s">
+        <v>68</v>
+      </c>
+      <c r="H49" t="s">
+        <v>172</v>
+      </c>
+      <c r="I49" s="1">
+        <v>37364</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>150</v>
+      </c>
+      <c r="D50" t="s">
+        <v>190</v>
+      </c>
+      <c r="E50" t="s">
+        <v>187</v>
+      </c>
+      <c r="F50" t="s">
+        <v>183</v>
+      </c>
+      <c r="G50" t="s">
+        <v>25</v>
+      </c>
+      <c r="H50" t="s">
+        <v>173</v>
+      </c>
+      <c r="I50" s="1">
+        <v>37930</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" t="s">
+        <v>192</v>
+      </c>
+      <c r="E51" t="s">
+        <v>186</v>
+      </c>
+      <c r="F51" t="s">
+        <v>184</v>
+      </c>
+      <c r="G51" t="s">
+        <v>177</v>
+      </c>
+      <c r="H51" t="s">
+        <v>174</v>
+      </c>
+      <c r="I51" s="1">
+        <v>37390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New episode draft and updated boards
</commit_message>
<xml_diff>
--- a/master_files/2023_draft_big_boards.xlsx
+++ b/master_files/2023_draft_big_boards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Bushman\Documents\R\jabber-jazz-content-notes\master_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3B3F2B-ED00-4835-937E-611D8BB5C913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9D8C50-A30C-462A-A02F-99A5D0F767D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11470" yWindow="0" windowWidth="7820" windowHeight="10170" firstSheet="4" activeTab="4" xr2:uid="{3F3E3C4B-A1D3-4C9C-9B2F-6D892D359046}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="5" xr2:uid="{3F3E3C4B-A1D3-4C9C-9B2F-6D892D359046}"/>
   </bookViews>
   <sheets>
     <sheet name="Josh-Roberts" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Mark" sheetId="3" r:id="rId3"/>
     <sheet name="AJ" sheetId="4" r:id="rId4"/>
     <sheet name="Adam-Bushman" sheetId="5" r:id="rId5"/>
+    <sheet name="Adam-Bushman-2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="212">
   <si>
     <t>pick</t>
   </si>
@@ -619,6 +620,63 @@
   </si>
   <si>
     <t>Off:Big</t>
+  </si>
+  <si>
+    <t>Jaylen Clark</t>
+  </si>
+  <si>
+    <t>Ben Sheppard</t>
+  </si>
+  <si>
+    <t>Omari Moore</t>
+  </si>
+  <si>
+    <t>Mike Miles Jr.</t>
+  </si>
+  <si>
+    <t>Olivier-Maxence Prosper</t>
+  </si>
+  <si>
+    <t>Belmont</t>
+  </si>
+  <si>
+    <t>San Jose State</t>
+  </si>
+  <si>
+    <t>TCU</t>
+  </si>
+  <si>
+    <t>Marquette</t>
+  </si>
+  <si>
+    <t>251 lbs</t>
+  </si>
+  <si>
+    <t>191 lbs</t>
+  </si>
+  <si>
+    <t>189 lbs</t>
+  </si>
+  <si>
+    <t>212 lbs</t>
+  </si>
+  <si>
+    <t>Wing</t>
+  </si>
+  <si>
+    <t>Big</t>
+  </si>
+  <si>
+    <t>Guard</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>194 lbs</t>
+  </si>
+  <si>
+    <t>7'4"</t>
   </si>
 </sst>
 </file>
@@ -4579,7 +4637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C80E46-0F5C-4BF5-9546-9B686A8E86D5}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -6071,4 +6129,1330 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA4F1CE9-658C-4042-9EB7-3E001B911D6D}">
+  <dimension ref="A1:I45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" t="s">
+        <v>211</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1">
+        <v>37990</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="1">
+        <v>37582</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="1">
+        <v>38020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>152</v>
+      </c>
+      <c r="I5" s="1">
+        <v>37868</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>206</v>
+      </c>
+      <c r="E6" t="s">
+        <v>209</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6" s="1">
+        <v>38176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I7" s="1">
+        <v>37651</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" t="s">
+        <v>154</v>
+      </c>
+      <c r="I8" s="1">
+        <v>37651</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9" t="s">
+        <v>208</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" s="1">
+        <v>38006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" t="s">
+        <v>176</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="1">
+        <v>37932</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E11" t="s">
+        <v>209</v>
+      </c>
+      <c r="F11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I11" s="1">
+        <v>37947</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12" t="s">
+        <v>208</v>
+      </c>
+      <c r="F12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" t="s">
+        <v>155</v>
+      </c>
+      <c r="I12" s="1">
+        <v>37791</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13" t="s">
+        <v>208</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" t="s">
+        <v>156</v>
+      </c>
+      <c r="I13" s="1">
+        <v>37885</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E14" t="s">
+        <v>206</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" t="s">
+        <v>155</v>
+      </c>
+      <c r="I14" s="1">
+        <v>38200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" t="s">
+        <v>206</v>
+      </c>
+      <c r="E15" t="s">
+        <v>206</v>
+      </c>
+      <c r="F15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="1">
+        <v>37464</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>208</v>
+      </c>
+      <c r="E16" t="s">
+        <v>208</v>
+      </c>
+      <c r="F16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="1">
+        <v>37933</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>206</v>
+      </c>
+      <c r="E17" t="s">
+        <v>209</v>
+      </c>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" t="s">
+        <v>154</v>
+      </c>
+      <c r="I17" s="1">
+        <v>38338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
+        <v>209</v>
+      </c>
+      <c r="E18" t="s">
+        <v>209</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18" s="1">
+        <v>37951</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" t="s">
+        <v>206</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="1">
+        <v>37878</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" t="s">
+        <v>208</v>
+      </c>
+      <c r="E20" t="s">
+        <v>208</v>
+      </c>
+      <c r="F20" t="s">
+        <v>127</v>
+      </c>
+      <c r="G20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" t="s">
+        <v>157</v>
+      </c>
+      <c r="I20" s="1">
+        <v>37375</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" t="s">
+        <v>206</v>
+      </c>
+      <c r="E21" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21" t="s">
+        <v>141</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" t="s">
+        <v>210</v>
+      </c>
+      <c r="I21" s="1">
+        <v>38194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>208</v>
+      </c>
+      <c r="E22" t="s">
+        <v>206</v>
+      </c>
+      <c r="F22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" t="s">
+        <v>158</v>
+      </c>
+      <c r="I22" s="1">
+        <v>37945</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E23" t="s">
+        <v>207</v>
+      </c>
+      <c r="F23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23" t="s">
+        <v>132</v>
+      </c>
+      <c r="I23" s="1">
+        <v>38029</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" t="s">
+        <v>209</v>
+      </c>
+      <c r="E24" t="s">
+        <v>209</v>
+      </c>
+      <c r="F24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" t="s">
+        <v>159</v>
+      </c>
+      <c r="I24" s="1">
+        <v>38079</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" t="s">
+        <v>206</v>
+      </c>
+      <c r="E25" t="s">
+        <v>206</v>
+      </c>
+      <c r="F25" t="s">
+        <v>118</v>
+      </c>
+      <c r="G25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25" s="1">
+        <v>37924</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>208</v>
+      </c>
+      <c r="E26" t="s">
+        <v>208</v>
+      </c>
+      <c r="F26" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" t="s">
+        <v>35</v>
+      </c>
+      <c r="I26" s="1">
+        <v>38095</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" t="s">
+        <v>208</v>
+      </c>
+      <c r="E27" t="s">
+        <v>206</v>
+      </c>
+      <c r="F27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" t="s">
+        <v>160</v>
+      </c>
+      <c r="I27" s="1">
+        <v>37404</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" t="s">
+        <v>209</v>
+      </c>
+      <c r="E28" t="s">
+        <v>209</v>
+      </c>
+      <c r="F28" t="s">
+        <v>178</v>
+      </c>
+      <c r="G28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" t="s">
+        <v>82</v>
+      </c>
+      <c r="I28" s="1">
+        <v>36757</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" t="s">
+        <v>207</v>
+      </c>
+      <c r="E29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F29" t="s">
+        <v>142</v>
+      </c>
+      <c r="G29" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" t="s">
+        <v>202</v>
+      </c>
+      <c r="I29" s="1">
+        <v>38213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" t="s">
+        <v>209</v>
+      </c>
+      <c r="E30" t="s">
+        <v>209</v>
+      </c>
+      <c r="F30" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" t="s">
+        <v>161</v>
+      </c>
+      <c r="I30" s="1">
+        <v>37208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" t="s">
+        <v>206</v>
+      </c>
+      <c r="E31" t="s">
+        <v>206</v>
+      </c>
+      <c r="F31" t="s">
+        <v>143</v>
+      </c>
+      <c r="G31" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" t="s">
+        <v>158</v>
+      </c>
+      <c r="I31" s="1">
+        <v>37677</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>193</v>
+      </c>
+      <c r="D32" t="s">
+        <v>206</v>
+      </c>
+      <c r="E32" t="s">
+        <v>206</v>
+      </c>
+      <c r="F32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" t="s">
+        <v>53</v>
+      </c>
+      <c r="H32" t="s">
+        <v>158</v>
+      </c>
+      <c r="I32" s="1">
+        <v>37177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" t="s">
+        <v>208</v>
+      </c>
+      <c r="E33" t="s">
+        <v>208</v>
+      </c>
+      <c r="F33" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" t="s">
+        <v>97</v>
+      </c>
+      <c r="H33" t="s">
+        <v>162</v>
+      </c>
+      <c r="I33" s="1">
+        <v>36790</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34" t="s">
+        <v>208</v>
+      </c>
+      <c r="E34" t="s">
+        <v>208</v>
+      </c>
+      <c r="F34" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" t="s">
+        <v>176</v>
+      </c>
+      <c r="H34" t="s">
+        <v>163</v>
+      </c>
+      <c r="I34" s="1">
+        <v>37621</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" t="s">
+        <v>209</v>
+      </c>
+      <c r="E35" t="s">
+        <v>209</v>
+      </c>
+      <c r="F35" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H35" t="s">
+        <v>121</v>
+      </c>
+      <c r="I35" s="1">
+        <v>38182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>194</v>
+      </c>
+      <c r="D36" t="s">
+        <v>208</v>
+      </c>
+      <c r="E36" t="s">
+        <v>206</v>
+      </c>
+      <c r="F36" t="s">
+        <v>198</v>
+      </c>
+      <c r="G36" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" s="1">
+        <v>36907</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" t="s">
+        <v>206</v>
+      </c>
+      <c r="E37" t="s">
+        <v>206</v>
+      </c>
+      <c r="F37" t="s">
+        <v>122</v>
+      </c>
+      <c r="G37" t="s">
+        <v>68</v>
+      </c>
+      <c r="H37" t="s">
+        <v>164</v>
+      </c>
+      <c r="I37" s="1">
+        <v>38138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
+        <v>208</v>
+      </c>
+      <c r="E38" t="s">
+        <v>208</v>
+      </c>
+      <c r="F38" t="s">
+        <v>94</v>
+      </c>
+      <c r="G38" t="s">
+        <v>176</v>
+      </c>
+      <c r="H38" t="s">
+        <v>203</v>
+      </c>
+      <c r="I38" s="1">
+        <v>38034</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>195</v>
+      </c>
+      <c r="D39" t="s">
+        <v>208</v>
+      </c>
+      <c r="E39" t="s">
+        <v>208</v>
+      </c>
+      <c r="F39" t="s">
+        <v>199</v>
+      </c>
+      <c r="G39" t="s">
+        <v>34</v>
+      </c>
+      <c r="H39" t="s">
+        <v>204</v>
+      </c>
+      <c r="I39" s="1">
+        <v>36787</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" t="s">
+        <v>206</v>
+      </c>
+      <c r="E40" t="s">
+        <v>206</v>
+      </c>
+      <c r="F40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G40" t="s">
+        <v>34</v>
+      </c>
+      <c r="H40" t="s">
+        <v>165</v>
+      </c>
+      <c r="I40" s="1">
+        <v>37106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" t="s">
+        <v>207</v>
+      </c>
+      <c r="E41" t="s">
+        <v>207</v>
+      </c>
+      <c r="F41" t="s">
+        <v>81</v>
+      </c>
+      <c r="G41" t="s">
+        <v>46</v>
+      </c>
+      <c r="H41" t="s">
+        <v>166</v>
+      </c>
+      <c r="I41" s="1">
+        <v>36578</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>196</v>
+      </c>
+      <c r="D42" t="s">
+        <v>208</v>
+      </c>
+      <c r="E42" t="s">
+        <v>208</v>
+      </c>
+      <c r="F42" t="s">
+        <v>200</v>
+      </c>
+      <c r="G42" t="s">
+        <v>97</v>
+      </c>
+      <c r="H42" t="s">
+        <v>117</v>
+      </c>
+      <c r="I42" s="1">
+        <v>37492</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" t="s">
+        <v>206</v>
+      </c>
+      <c r="E43" t="s">
+        <v>209</v>
+      </c>
+      <c r="F43" t="s">
+        <v>61</v>
+      </c>
+      <c r="G43" t="s">
+        <v>68</v>
+      </c>
+      <c r="H43" t="s">
+        <v>132</v>
+      </c>
+      <c r="I43" s="1">
+        <v>36834</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D44" t="s">
+        <v>209</v>
+      </c>
+      <c r="E44" t="s">
+        <v>209</v>
+      </c>
+      <c r="F44" t="s">
+        <v>94</v>
+      </c>
+      <c r="G44" t="s">
+        <v>68</v>
+      </c>
+      <c r="H44" t="s">
+        <v>167</v>
+      </c>
+      <c r="I44" s="1">
+        <v>36940</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>197</v>
+      </c>
+      <c r="D45" t="s">
+        <v>209</v>
+      </c>
+      <c r="E45" t="s">
+        <v>209</v>
+      </c>
+      <c r="F45" t="s">
+        <v>201</v>
+      </c>
+      <c r="G45" t="s">
+        <v>25</v>
+      </c>
+      <c r="H45" t="s">
+        <v>205</v>
+      </c>
+      <c r="I45" s="1">
+        <v>37440</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>